<commit_message>
take entry and create stop loss
</commit_message>
<xml_diff>
--- a/BNFStragleTestReport.xlsx
+++ b/BNFStragleTestReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
   <si>
     <t>DATE</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>2022-07-05</t>
+  </si>
+  <si>
+    <t>2022-07-06</t>
+  </si>
+  <si>
+    <t>2022-07-07</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1020,6 +1026,40 @@
         <v>249.99999999999983</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="n">
+        <v>6.100000000000001</v>
+      </c>
+      <c r="D48" t="n">
+        <v>152.50000000000003</v>
+      </c>
+      <c r="E48" t="n">
+        <v>610.0000000000001</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" t="n">
+        <v>36.45</v>
+      </c>
+      <c r="D49" t="n">
+        <v>911.2500000000001</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3645.0000000000005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>